<commit_message>
standardized Multi KDMA in definition files
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/SurveyResults/Exploratory Delegation Variables - PH2.xlsx
+++ b/dashboard-ui/src/components/SurveyResults/Exploratory Delegation Variables - PH2.xlsx
@@ -1,32 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C9A49A1-DD22-4AC0-85D9-12FE8835B45A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -189,7 +172,7 @@
     <t>The participant's response to "How much experience did you have with VR Gaming before today?"</t>
   </si>
   <si>
-    <t>X refers to the block number, Y refers to the DM number the participant saw. For Eval 8 and 9, participants saw 4 blocks with 3-4 DMs each (4 in the case of multi-kdma). The following columns describe each page of the survey using this BX_DMY format.</t>
+    <t>X refers to the block number, Y refers to the DM number the participant saw. For Eval 8 and 9, participants saw 4 blocks with 3-4 DMs each (4 in the case of Multi KDMA). The following columns describe each page of the survey using this BX_DMY format.</t>
   </si>
   <si>
     <t>The alignment level of the DM based on the alignment gathered from the participant's text responses</t>
@@ -234,7 +217,7 @@
     <t>The name and alignment value of the third medic being compared in this comparison page</t>
   </si>
   <si>
-    <t>The name and alignment value of the fourth medic being compared in this comparison page - only applies to multi-kdma</t>
+    <t>The name and alignment value of the fourth medic being compared in this comparison page - only applies to Multi KDMA</t>
   </si>
   <si>
     <t>The amount of time the participant spent (Minutes) on the comparison page</t>
@@ -243,7 +226,7 @@
     <t>The alignment of the first two DMs being compared</t>
   </si>
   <si>
-    <t>The response to the first forced choice question (baseline vs aligned, or follow the previous column for multikdma)</t>
+    <t>The response to the first forced choice question (baseline vs aligned, or follow the previous column for Multi KDMA)</t>
   </si>
   <si>
     <t>The response to "Rate your confidence about the delegation decision indicated in the previous question" for the first forced choice</t>
@@ -252,22 +235,22 @@
     <t>The participant's explanation for their delegation choice</t>
   </si>
   <si>
-    <t>The difference between the Delegator|Observed_ADM alignment comparison between the aligned ADM and the baseline ADM (or whatever is in the Alignment column for multikdma)</t>
+    <t>The difference between the Delegator|Observed_ADM alignment comparison between the aligned ADM and the baseline ADM (or whatever is in the Alignment column for Multi KDMA)</t>
   </si>
   <si>
     <t>The alignment of the second two DMs being compared</t>
   </si>
   <si>
-    <t>The response to the second forced choice question (aligned vs misaligned, or follow the previous column for multikdma)</t>
+    <t>The response to the second forced choice question (aligned vs misaligned, or follow the previous column for Multi KDMA)</t>
   </si>
   <si>
     <t>The response to "Rate your confidence about the delegation decision indicated in the previous question" for the second forced choice question</t>
   </si>
   <si>
-    <t>The difference between the Delegator|Observed_ADM alignment comparison between the aligned ADM and the misaligned ADM (or follow the alignment column for multikdma)</t>
-  </si>
-  <si>
-    <t>The alignment of the third two DMs being compared (multikdma only)</t>
+    <t>The difference between the Delegator|Observed_ADM alignment comparison between the aligned ADM and the misaligned ADM (or follow the alignment column for Multi KDMA)</t>
+  </si>
+  <si>
+    <t>The alignment of the third two DMs being compared (Multi KDMA only)</t>
   </si>
   <si>
     <t>The response to the third forced choice question (follow the previous column)</t>
@@ -286,6 +269,9 @@
   </si>
   <si>
     <r>
+      <t/>
+    </r>
+    <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
@@ -298,7 +284,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -318,7 +304,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -338,7 +324,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -358,7 +344,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -396,6 +382,9 @@
   </si>
   <si>
     <r>
+      <t/>
+    </r>
+    <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
@@ -408,7 +397,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -428,7 +417,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -448,7 +437,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -468,7 +457,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -488,6 +477,9 @@
   </si>
   <si>
     <r>
+      <t/>
+    </r>
+    <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
@@ -500,7 +492,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -520,7 +512,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -540,7 +532,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -560,7 +552,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -580,6 +572,9 @@
   </si>
   <si>
     <r>
+      <t/>
+    </r>
+    <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
@@ -592,7 +587,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -612,7 +607,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -632,7 +627,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -652,7 +647,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -672,6 +667,9 @@
   </si>
   <si>
     <r>
+      <t/>
+    </r>
+    <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
@@ -684,7 +682,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -704,7 +702,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -724,7 +722,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -744,7 +742,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -767,6 +765,9 @@
   </si>
   <si>
     <r>
+      <t/>
+    </r>
+    <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
@@ -779,7 +780,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -799,7 +800,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -819,7 +820,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -839,7 +840,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -859,6 +860,9 @@
   </si>
   <si>
     <r>
+      <t/>
+    </r>
+    <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
@@ -871,7 +875,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -891,7 +895,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -911,7 +915,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -931,7 +935,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -956,8 +960,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -973,23 +978,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF212529"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1019,45 +1016,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="8">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1068,10 +1058,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1109,71 +1099,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1201,7 +1191,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1224,11 +1214,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1237,13 +1227,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1253,7 +1243,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1262,7 +1252,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1271,7 +1261,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1279,10 +1269,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1347,52 +1337,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:AS3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AQ3" sqref="AQ3"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" style="5" customWidth="1"/>
-    <col min="14" max="16" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.140625" style="5" customWidth="1"/>
-    <col min="28" max="28" width="19.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.42578125" style="5" customWidth="1"/>
-    <col min="30" max="30" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="25.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.7109375" style="5" customWidth="1"/>
-    <col min="35" max="35" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="23" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="24.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="42" width="32.140625" customWidth="1"/>
-    <col min="43" max="43" width="38.7109375" customWidth="1"/>
+    <col min="1" max="1" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="7" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="6" width="19.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="6" width="20.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="6" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="6" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="6" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="6" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="6" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="6" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="6" width="22.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="6" width="25.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="6" width="25.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="6" width="18.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="6" width="23.005" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="6" width="24.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="6" width="32.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="6" width="32.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="41" max="41" style="6" width="32.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="42" max="42" style="6" width="32.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="43" max="43" style="6" width="38.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="44" max="44" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="45" max="45" style="7" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="1" customFormat="1" ht="60" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="66" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1426,25 +1428,25 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="2" t="s">
@@ -1471,13 +1473,13 @@
       <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
       <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
       <c r="AD1" s="2" t="s">
@@ -1492,10 +1494,10 @@
       <c r="AG1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="7" t="s">
+      <c r="AH1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="7" t="s">
+      <c r="AI1" s="2" t="s">
         <v>34</v>
       </c>
       <c r="AJ1" s="2" t="s">
@@ -1507,16 +1509,16 @@
       <c r="AL1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="7" t="s">
+      <c r="AM1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="7" t="s">
+      <c r="AN1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="7" t="s">
+      <c r="AO1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="7" t="s">
+      <c r="AP1" s="2" t="s">
         <v>41</v>
       </c>
       <c r="AQ1" s="2" t="s">
@@ -1525,7 +1527,7 @@
       <c r="AR1" s="3"/>
       <c r="AS1" s="3"/>
     </row>
-    <row r="2" spans="1:45" s="1" customFormat="1" ht="249" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="222.75" customFormat="1" s="1">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -1556,26 +1558,26 @@
       <c r="J2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7" t="s">
+      <c r="M2" s="2"/>
+      <c r="N2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="2" t="s">
         <v>56</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="2" t="s">
         <v>58</v>
       </c>
       <c r="S2" s="2" t="s">
@@ -1602,16 +1604,16 @@
       <c r="Z2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AA2" s="7" t="s">
+      <c r="AA2" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AB2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AC2" s="7" t="s">
+      <c r="AC2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="AD2" s="7" t="s">
+      <c r="AD2" s="2" t="s">
         <v>70</v>
       </c>
       <c r="AE2" s="2" t="s">
@@ -1623,10 +1625,10 @@
       <c r="AG2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AH2" s="7" t="s">
+      <c r="AH2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AI2" s="7" t="s">
+      <c r="AI2" s="2" t="s">
         <v>75</v>
       </c>
       <c r="AJ2" s="2" t="s">
@@ -1638,16 +1640,16 @@
       <c r="AL2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AM2" s="7" t="s">
+      <c r="AM2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AN2" s="7" t="s">
+      <c r="AN2" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AO2" s="7" t="s">
+      <c r="AO2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AP2" s="7" t="s">
+      <c r="AP2" s="2" t="s">
         <v>72</v>
       </c>
       <c r="AQ2" s="2" t="s">
@@ -1656,7 +1658,7 @@
       <c r="AR2" s="3"/>
       <c r="AS2" s="3"/>
     </row>
-    <row r="3" spans="1:45" s="1" customFormat="1" ht="114" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="133.5" customFormat="1" s="1">
       <c r="A3" s="2" t="s">
         <v>82</v>
       </c>
@@ -1676,21 +1678,21 @@
       <c r="K3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="P3" s="7"/>
+      <c r="P3" s="2"/>
       <c r="Q3" s="3"/>
-      <c r="R3" s="9" t="s">
+      <c r="R3" s="2" t="s">
         <v>90</v>
       </c>
       <c r="S3" s="2" t="s">
@@ -1711,17 +1713,17 @@
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
-      <c r="AA3" s="7"/>
+      <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
-      <c r="AC3" s="7"/>
+      <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="2" t="s">
         <v>96</v>
       </c>
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
-      <c r="AH3" s="7"/>
-      <c r="AI3" s="7"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
       <c r="AJ3" s="2" t="s">
         <v>97</v>
       </c>
@@ -1731,12 +1733,12 @@
       <c r="AL3" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="AM3" s="7"/>
-      <c r="AN3" s="7"/>
-      <c r="AO3" s="7" t="s">
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="AP3" s="7"/>
+      <c r="AP3" s="2"/>
       <c r="AQ3" s="2" t="s">
         <v>98</v>
       </c>

</xml_diff>

<commit_message>
standardized Multi KDMA in definition files (#335)
</commit_message>
<xml_diff>
--- a/dashboard-ui/src/components/SurveyResults/Exploratory Delegation Variables - PH2.xlsx
+++ b/dashboard-ui/src/components/SurveyResults/Exploratory Delegation Variables - PH2.xlsx
@@ -1,32 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C9A49A1-DD22-4AC0-85D9-12FE8835B45A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -189,7 +172,7 @@
     <t>The participant's response to "How much experience did you have with VR Gaming before today?"</t>
   </si>
   <si>
-    <t>X refers to the block number, Y refers to the DM number the participant saw. For Eval 8 and 9, participants saw 4 blocks with 3-4 DMs each (4 in the case of multi-kdma). The following columns describe each page of the survey using this BX_DMY format.</t>
+    <t>X refers to the block number, Y refers to the DM number the participant saw. For Eval 8 and 9, participants saw 4 blocks with 3-4 DMs each (4 in the case of Multi KDMA). The following columns describe each page of the survey using this BX_DMY format.</t>
   </si>
   <si>
     <t>The alignment level of the DM based on the alignment gathered from the participant's text responses</t>
@@ -234,7 +217,7 @@
     <t>The name and alignment value of the third medic being compared in this comparison page</t>
   </si>
   <si>
-    <t>The name and alignment value of the fourth medic being compared in this comparison page - only applies to multi-kdma</t>
+    <t>The name and alignment value of the fourth medic being compared in this comparison page - only applies to Multi KDMA</t>
   </si>
   <si>
     <t>The amount of time the participant spent (Minutes) on the comparison page</t>
@@ -243,7 +226,7 @@
     <t>The alignment of the first two DMs being compared</t>
   </si>
   <si>
-    <t>The response to the first forced choice question (baseline vs aligned, or follow the previous column for multikdma)</t>
+    <t>The response to the first forced choice question (baseline vs aligned, or follow the previous column for Multi KDMA)</t>
   </si>
   <si>
     <t>The response to "Rate your confidence about the delegation decision indicated in the previous question" for the first forced choice</t>
@@ -252,22 +235,22 @@
     <t>The participant's explanation for their delegation choice</t>
   </si>
   <si>
-    <t>The difference between the Delegator|Observed_ADM alignment comparison between the aligned ADM and the baseline ADM (or whatever is in the Alignment column for multikdma)</t>
+    <t>The difference between the Delegator|Observed_ADM alignment comparison between the aligned ADM and the baseline ADM (or whatever is in the Alignment column for Multi KDMA)</t>
   </si>
   <si>
     <t>The alignment of the second two DMs being compared</t>
   </si>
   <si>
-    <t>The response to the second forced choice question (aligned vs misaligned, or follow the previous column for multikdma)</t>
+    <t>The response to the second forced choice question (aligned vs misaligned, or follow the previous column for Multi KDMA)</t>
   </si>
   <si>
     <t>The response to "Rate your confidence about the delegation decision indicated in the previous question" for the second forced choice question</t>
   </si>
   <si>
-    <t>The difference between the Delegator|Observed_ADM alignment comparison between the aligned ADM and the misaligned ADM (or follow the alignment column for multikdma)</t>
-  </si>
-  <si>
-    <t>The alignment of the third two DMs being compared (multikdma only)</t>
+    <t>The difference between the Delegator|Observed_ADM alignment comparison between the aligned ADM and the misaligned ADM (or follow the alignment column for Multi KDMA)</t>
+  </si>
+  <si>
+    <t>The alignment of the third two DMs being compared (Multi KDMA only)</t>
   </si>
   <si>
     <t>The response to the third forced choice question (follow the previous column)</t>
@@ -286,6 +269,9 @@
   </si>
   <si>
     <r>
+      <t/>
+    </r>
+    <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
@@ -298,7 +284,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -318,7 +304,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -338,7 +324,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -358,7 +344,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -396,6 +382,9 @@
   </si>
   <si>
     <r>
+      <t/>
+    </r>
+    <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
@@ -408,7 +397,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -428,7 +417,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -448,7 +437,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -468,7 +457,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -488,6 +477,9 @@
   </si>
   <si>
     <r>
+      <t/>
+    </r>
+    <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
@@ -500,7 +492,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -520,7 +512,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -540,7 +532,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -560,7 +552,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -580,6 +572,9 @@
   </si>
   <si>
     <r>
+      <t/>
+    </r>
+    <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
@@ -592,7 +587,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -612,7 +607,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -632,7 +627,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -652,7 +647,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -672,6 +667,9 @@
   </si>
   <si>
     <r>
+      <t/>
+    </r>
+    <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
@@ -684,7 +682,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -704,7 +702,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -724,7 +722,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -744,7 +742,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -767,6 +765,9 @@
   </si>
   <si>
     <r>
+      <t/>
+    </r>
+    <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
@@ -779,7 +780,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -799,7 +800,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -819,7 +820,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -839,7 +840,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -859,6 +860,9 @@
   </si>
   <si>
     <r>
+      <t/>
+    </r>
+    <r>
       <rPr>
         <sz val="11"/>
         <color rgb="FF000000"/>
@@ -871,7 +875,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -891,7 +895,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -911,7 +915,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -931,7 +935,7 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFFFFFF"/>
+        <color rgb="FFffffff"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -956,8 +960,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -973,23 +978,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF212529"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1019,45 +1016,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="8">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1068,10 +1058,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1109,71 +1099,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1201,7 +1191,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1224,11 +1214,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1237,13 +1227,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1253,7 +1243,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1262,7 +1252,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1271,7 +1261,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1279,10 +1269,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1347,52 +1337,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:AS3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
-      <selection activeCell="AQ3" sqref="AQ3"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.7109375" style="5" customWidth="1"/>
-    <col min="14" max="16" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="20.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="18.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="18.140625" style="5" customWidth="1"/>
-    <col min="28" max="28" width="19.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.42578125" style="5" customWidth="1"/>
-    <col min="30" max="30" width="16.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="25.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="25.7109375" style="5" customWidth="1"/>
-    <col min="35" max="35" width="18.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="23" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="24.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="42" width="32.140625" customWidth="1"/>
-    <col min="43" max="43" width="38.7109375" customWidth="1"/>
+    <col min="1" max="1" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="7" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" style="7" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" style="6" width="19.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="20" max="20" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="6" width="20.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="22" max="22" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="23" max="23" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="24" max="24" style="6" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="25" max="25" style="6" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="26" max="26" style="6" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="27" max="27" style="6" width="18.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="28" max="28" style="6" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="29" max="29" style="6" width="19.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="30" max="30" style="6" width="16.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="31" max="31" style="6" width="22.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="32" max="32" style="6" width="25.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="33" max="33" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="34" max="34" style="6" width="25.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="35" max="35" style="6" width="18.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="36" max="36" style="6" width="23.005" customWidth="1" bestFit="1"/>
+    <col min="37" max="37" style="6" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="38" max="38" style="6" width="24.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="39" max="39" style="6" width="32.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="40" max="40" style="6" width="32.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="41" max="41" style="6" width="32.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="42" max="42" style="6" width="32.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="43" max="43" style="6" width="38.71928571428572" customWidth="1" bestFit="1"/>
+    <col min="44" max="44" style="7" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="45" max="45" style="7" width="13.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" s="1" customFormat="1" ht="60" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="66" customFormat="1" s="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1426,25 +1428,25 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="7" t="s">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="7" t="s">
+      <c r="R1" s="2" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="2" t="s">
@@ -1471,13 +1473,13 @@
       <c r="Z1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AA1" s="2" t="s">
         <v>26</v>
       </c>
       <c r="AB1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AC1" s="2" t="s">
         <v>28</v>
       </c>
       <c r="AD1" s="2" t="s">
@@ -1492,10 +1494,10 @@
       <c r="AG1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="7" t="s">
+      <c r="AH1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="7" t="s">
+      <c r="AI1" s="2" t="s">
         <v>34</v>
       </c>
       <c r="AJ1" s="2" t="s">
@@ -1507,16 +1509,16 @@
       <c r="AL1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="7" t="s">
+      <c r="AM1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="7" t="s">
+      <c r="AN1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="7" t="s">
+      <c r="AO1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="7" t="s">
+      <c r="AP1" s="2" t="s">
         <v>41</v>
       </c>
       <c r="AQ1" s="2" t="s">
@@ -1525,7 +1527,7 @@
       <c r="AR1" s="3"/>
       <c r="AS1" s="3"/>
     </row>
-    <row r="2" spans="1:45" s="1" customFormat="1" ht="249" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="222.75" customFormat="1" s="1">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -1556,26 +1558,26 @@
       <c r="J2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="K2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="L2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="M2" s="7"/>
-      <c r="N2" s="7" t="s">
+      <c r="M2" s="2"/>
+      <c r="N2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="O2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="P2" s="2" t="s">
         <v>56</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="R2" s="2" t="s">
         <v>58</v>
       </c>
       <c r="S2" s="2" t="s">
@@ -1602,16 +1604,16 @@
       <c r="Z2" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AA2" s="7" t="s">
+      <c r="AA2" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AB2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AC2" s="7" t="s">
+      <c r="AC2" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="AD2" s="7" t="s">
+      <c r="AD2" s="2" t="s">
         <v>70</v>
       </c>
       <c r="AE2" s="2" t="s">
@@ -1623,10 +1625,10 @@
       <c r="AG2" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="AH2" s="7" t="s">
+      <c r="AH2" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="AI2" s="7" t="s">
+      <c r="AI2" s="2" t="s">
         <v>75</v>
       </c>
       <c r="AJ2" s="2" t="s">
@@ -1638,16 +1640,16 @@
       <c r="AL2" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="AM2" s="7" t="s">
+      <c r="AM2" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="AN2" s="7" t="s">
+      <c r="AN2" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AO2" s="7" t="s">
+      <c r="AO2" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="AP2" s="7" t="s">
+      <c r="AP2" s="2" t="s">
         <v>72</v>
       </c>
       <c r="AQ2" s="2" t="s">
@@ -1656,7 +1658,7 @@
       <c r="AR2" s="3"/>
       <c r="AS2" s="3"/>
     </row>
-    <row r="3" spans="1:45" s="1" customFormat="1" ht="114" customHeight="1">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="133.5" customFormat="1" s="1">
       <c r="A3" s="2" t="s">
         <v>82</v>
       </c>
@@ -1676,21 +1678,21 @@
       <c r="K3" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="M3" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="N3" s="8" t="s">
+      <c r="N3" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="O3" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="P3" s="7"/>
+      <c r="P3" s="2"/>
       <c r="Q3" s="3"/>
-      <c r="R3" s="9" t="s">
+      <c r="R3" s="2" t="s">
         <v>90</v>
       </c>
       <c r="S3" s="2" t="s">
@@ -1711,17 +1713,17 @@
       <c r="X3" s="2"/>
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
-      <c r="AA3" s="7"/>
+      <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
-      <c r="AC3" s="7"/>
+      <c r="AC3" s="2"/>
       <c r="AD3" s="2"/>
       <c r="AE3" s="2" t="s">
         <v>96</v>
       </c>
       <c r="AF3" s="2"/>
       <c r="AG3" s="2"/>
-      <c r="AH3" s="7"/>
-      <c r="AI3" s="7"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
       <c r="AJ3" s="2" t="s">
         <v>97</v>
       </c>
@@ -1731,12 +1733,12 @@
       <c r="AL3" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="AM3" s="7"/>
-      <c r="AN3" s="7"/>
-      <c r="AO3" s="7" t="s">
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="AP3" s="7"/>
+      <c r="AP3" s="2"/>
       <c r="AQ3" s="2" t="s">
         <v>98</v>
       </c>

</xml_diff>